<commit_message>
Optimisation de l'heurisique destructrice.
</commit_message>
<xml_diff>
--- a/Bnechmark2 avec voisinnage.xlsx
+++ b/Bnechmark2 avec voisinnage.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\Ecole\MetaHeu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\MPRO\MH\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="out_1" localSheetId="0">Feuil1!$B$3:$O$8</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -209,12 +209,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -315,6 +315,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -350,6 +367,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -504,18 +538,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24:M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="2"/>
-    <col min="2" max="2" width="10.75" style="3"/>
-    <col min="3" max="16384" width="10.75" style="1"/>
+    <col min="1" max="1" width="10.77734375" style="2"/>
+    <col min="2" max="2" width="10.77734375" style="3"/>
+    <col min="3" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -532,41 +566,41 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B2" s="7">
         <v>10</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7">
         <v>15</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7">
         <v>20</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7">
         <v>25</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4">
+      <c r="I2" s="7"/>
+      <c r="J2" s="7">
         <v>30</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4">
+      <c r="K2" s="7"/>
+      <c r="L2" s="7">
         <v>40</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4">
+      <c r="M2" s="7"/>
+      <c r="N2" s="7">
         <v>50</v>
       </c>
-      <c r="O2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -609,11 +643,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>41</v>
       </c>
       <c r="C4" s="1">
@@ -656,11 +690,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>19</v>
       </c>
       <c r="C5" s="1">
@@ -703,11 +737,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -750,11 +784,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -797,11 +831,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>6</v>
       </c>
       <c r="C8" s="1">
@@ -844,43 +878,43 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
         <v>10</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7">
         <v>15</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4">
+      <c r="E11" s="7"/>
+      <c r="F11" s="7">
         <v>20</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4">
+      <c r="G11" s="7"/>
+      <c r="H11" s="7">
         <v>25</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4">
+      <c r="I11" s="7"/>
+      <c r="J11" s="7">
         <v>30</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4">
+      <c r="K11" s="7"/>
+      <c r="L11" s="7">
         <v>40</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4">
+      <c r="M11" s="7"/>
+      <c r="N11" s="7">
         <v>50</v>
       </c>
-      <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="3">
@@ -926,8 +960,8 @@
         <v>465</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="3">
@@ -973,8 +1007,8 @@
         <v>14.664999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="3">
@@ -1020,8 +1054,8 @@
         <v>1.633</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="3">
@@ -1067,8 +1101,8 @@
         <v>1.4390000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="3">
@@ -1114,8 +1148,8 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="3">
@@ -1161,290 +1195,325 @@
         <v>0.71799999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="7">
         <v>10</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7">
         <v>15</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4">
+      <c r="E20" s="7"/>
+      <c r="F20" s="7">
         <v>20</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4">
+      <c r="G20" s="7"/>
+      <c r="H20" s="7">
         <v>25</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4">
+      <c r="I20" s="7"/>
+      <c r="J20" s="7">
         <v>30</v>
       </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4">
+      <c r="K20" s="7"/>
+      <c r="L20" s="7">
         <v>40</v>
       </c>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4">
+      <c r="M20" s="7"/>
+      <c r="N20" s="7">
         <v>50</v>
       </c>
-      <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="O20" s="7"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <f>(B3-B12)/B3</f>
         <v>2.3809523809523808E-2</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7">
-        <f t="shared" ref="C21:O21" si="0">(D3-D12)/D3</f>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6">
+        <f t="shared" ref="D21:N21" si="0">(D3-D12)/D3</f>
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6">
         <f t="shared" si="0"/>
         <v>5.9880239520958084E-2</v>
       </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6">
         <f t="shared" si="0"/>
         <v>5.3846153846153849E-2</v>
       </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7">
+      <c r="I21" s="6"/>
+      <c r="J21" s="6">
         <f t="shared" si="0"/>
         <v>4.9450549450549448E-2</v>
       </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7">
+      <c r="K21" s="6"/>
+      <c r="L21" s="6">
         <f t="shared" si="0"/>
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7">
+      <c r="M21" s="6"/>
+      <c r="N21" s="6">
         <f t="shared" si="0"/>
         <v>2.9940119760479042E-2</v>
       </c>
-      <c r="O21" s="7"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <f t="shared" ref="B22:B26" si="1">(B4-B13)/B4</f>
         <v>0.21951219512195122</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7">
-        <f t="shared" ref="D22:O22" si="2">(D4-D13)/D4</f>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6">
+        <f t="shared" ref="D22" si="2">(D4-D13)/D4</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7">
-        <f t="shared" ref="F22:O22" si="3">(F4-F13)/F4</f>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6">
+        <f t="shared" ref="F22" si="3">(F4-F13)/F4</f>
         <v>0.36464088397790057</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7">
-        <f t="shared" ref="H22:O22" si="4">(H4-H13)/H4</f>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6">
+        <f t="shared" ref="H22" si="4">(H4-H13)/H4</f>
         <v>0.20085470085470086</v>
       </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7">
-        <f t="shared" ref="J22:O22" si="5">(J4-J13)/J4</f>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6">
+        <f t="shared" ref="J22" si="5">(J4-J13)/J4</f>
         <v>0.41330166270783847</v>
       </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7">
-        <f t="shared" ref="L22:O22" si="6">(L4-L13)/L4</f>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6">
+        <f t="shared" ref="L22" si="6">(L4-L13)/L4</f>
         <v>0.43495400788436267</v>
       </c>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7">
-        <f t="shared" ref="N22:O22" si="7">(N4-N13)/N4</f>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6">
+        <f t="shared" ref="N22" si="7">(N4-N13)/N4</f>
         <v>0.44879267277268942</v>
       </c>
-      <c r="O22" s="7"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <f t="shared" si="1"/>
         <v>0.10526315789473684</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7">
-        <f t="shared" ref="D23:O23" si="8">(D5-D14)/D5</f>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6">
+        <f t="shared" ref="D23" si="8">(D5-D14)/D5</f>
         <v>2.564102564102564E-2</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7">
-        <f t="shared" ref="F23:O23" si="9">(F5-F14)/F5</f>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6">
+        <f t="shared" ref="F23" si="9">(F5-F14)/F5</f>
         <v>0</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7">
-        <f t="shared" ref="H23:O23" si="10">(H5-H14)/H5</f>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6">
+        <f t="shared" ref="H23" si="10">(H5-H14)/H5</f>
         <v>7.0796460176991149E-2</v>
       </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7">
-        <f t="shared" ref="J23:O23" si="11">(J5-J14)/J5</f>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6">
+        <f t="shared" ref="J23" si="11">(J5-J14)/J5</f>
         <v>1.2903225806451613E-2</v>
       </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7">
-        <f t="shared" ref="L23:O23" si="12">(L5-L14)/L5</f>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6">
+        <f t="shared" ref="L23" si="12">(L5-L14)/L5</f>
         <v>5.9859154929577461E-2</v>
       </c>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7">
-        <f t="shared" ref="N23:O23" si="13">(N5-N14)/N5</f>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6">
+        <f t="shared" ref="N23" si="13">(N5-N14)/N5</f>
         <v>1.4598540145985401E-2</v>
       </c>
-      <c r="O23" s="7"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <f t="shared" si="1"/>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7">
-        <f t="shared" ref="D24:O24" si="14">(D6-D15)/D6</f>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6">
+        <f t="shared" ref="D24" si="14">(D6-D15)/D6</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7">
-        <f t="shared" ref="F24:O24" si="15">(F6-F15)/F6</f>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6">
+        <f t="shared" ref="F24" si="15">(F6-F15)/F6</f>
         <v>1.9607843137254902E-2</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7">
-        <f t="shared" ref="H24:O24" si="16">(H6-H15)/H6</f>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6">
+        <f t="shared" ref="H24" si="16">(H6-H15)/H6</f>
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7">
-        <f t="shared" ref="J24:O24" si="17">(J6-J15)/J6</f>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6">
+        <f t="shared" ref="J24" si="17">(J6-J15)/J6</f>
         <v>9.0090090090090089E-3</v>
       </c>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7">
-        <f t="shared" ref="L24:O24" si="18">(L6-L15)/L6</f>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6">
+        <f t="shared" ref="L24" si="18">(L6-L15)/L6</f>
         <v>2.5125628140703519E-2</v>
       </c>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7">
-        <f t="shared" ref="N24:O24" si="19">(N6-N15)/N6</f>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6">
+        <f t="shared" ref="N24" si="19">(N6-N15)/N6</f>
         <v>1.6286644951140065E-2</v>
       </c>
-      <c r="O24" s="7"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7">
-        <f t="shared" ref="D25:O25" si="20">(D7-D16)/D7</f>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6">
+        <f t="shared" ref="D25" si="20">(D7-D16)/D7</f>
         <v>9.5238095238095233E-2</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7">
-        <f t="shared" ref="F25:O25" si="21">(F7-F16)/F7</f>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6">
+        <f t="shared" ref="F25" si="21">(F7-F16)/F7</f>
         <v>5.7142857142857141E-2</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7">
-        <f t="shared" ref="H25:O25" si="22">(H7-H16)/H7</f>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6">
+        <f t="shared" ref="H25" si="22">(H7-H16)/H7</f>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7">
-        <f t="shared" ref="J25:O25" si="23">(J7-J16)/J7</f>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6">
+        <f t="shared" ref="J25" si="23">(J7-J16)/J7</f>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7">
-        <f t="shared" ref="L25:O25" si="24">(L7-L16)/L7</f>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6">
+        <f t="shared" ref="L25" si="24">(L7-L16)/L7</f>
         <v>3.5971223021582732E-2</v>
       </c>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7">
-        <f t="shared" ref="N25:O25" si="25">(N7-N16)/N7</f>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6">
+        <f t="shared" ref="N25" si="25">(N7-N16)/N7</f>
         <v>3.2407407407407406E-2</v>
       </c>
-      <c r="O25" s="7"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="O25" s="6"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7">
-        <f t="shared" ref="D26:O26" si="26">(D8-D17)/D8</f>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6">
+        <f t="shared" ref="D26" si="26">(D8-D17)/D8</f>
         <v>0</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7">
-        <f t="shared" ref="F26:O26" si="27">(F8-F17)/F8</f>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6">
+        <f t="shared" ref="F26" si="27">(F8-F17)/F8</f>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7">
-        <f t="shared" ref="H26:O26" si="28">(H8-H17)/H8</f>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6">
+        <f t="shared" ref="H26" si="28">(H8-H17)/H8</f>
         <v>2.3809523809523808E-2</v>
       </c>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7">
-        <f t="shared" ref="J26:O26" si="29">(J8-J17)/J8</f>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6">
+        <f t="shared" ref="J26" si="29">(J8-J17)/J8</f>
         <v>3.5087719298245612E-2</v>
       </c>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7">
-        <f t="shared" ref="L26:O26" si="30">(L8-L17)/L8</f>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6">
+        <f t="shared" ref="L26" si="30">(L8-L17)/L8</f>
         <v>1.9607843137254902E-2</v>
       </c>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7">
-        <f t="shared" ref="N26:O26" si="31">(N8-N17)/N8</f>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6">
+        <f t="shared" ref="N26" si="31">(N8-N17)/N8</f>
         <v>2.5316455696202531E-2</v>
       </c>
-      <c r="O26" s="7"/>
+      <c r="O26" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="L24:M24"/>
     <mergeCell ref="N24:O24"/>
     <mergeCell ref="B25:C25"/>
@@ -1459,48 +1528,13 @@
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>